<commit_message>
add GeoPolRisk for elementary flows
</commit_message>
<xml_diff>
--- a/dev/GeoPolRisk/results_elementary_flows.xlsx
+++ b/dev/GeoPolRisk/results_elementary_flows.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahnme_a\PycharmProjects\edges\dev\GeoPolRisk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9FE627-5B12-4E65-9DB1-E4F9191369C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E832CC79-0E3A-4CDA-8DDF-CD0331C37E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="136">
   <si>
     <t>Year</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Operator</t>
   </si>
   <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
     <t>Global</t>
   </si>
   <si>
@@ -382,15 +379,9 @@
     <t>Tantalum</t>
   </si>
   <si>
-    <t>bauxite</t>
-  </si>
-  <si>
     <t>startswith</t>
   </si>
   <si>
-    <t>Biosphere flow</t>
-  </si>
-  <si>
     <t>natural resource::in ground</t>
   </si>
   <si>
@@ -419,6 +410,24 @@
   </si>
   <si>
     <t>Coal, brown</t>
+  </si>
+  <si>
+    <t>Dataset name</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>280480</t>
+  </si>
+  <si>
+    <t>Arsenic</t>
+  </si>
+  <si>
+    <t>261210</t>
+  </si>
+  <si>
+    <t>Uranium</t>
   </si>
 </sst>
 </file>
@@ -430,14 +439,6 @@
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -477,6 +478,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -512,31 +519,22 @@
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma 2" xfId="6" xr:uid="{EFFD69F4-178D-429B-8956-5554E0F0062B}"/>
@@ -850,33 +848,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F1553C-43B9-4D9A-BC49-B6058EC3B2DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9C2F7F-2275-4806-82FF-371830C1A546}">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T41" sqref="T41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -928,7 +907,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>16</v>
@@ -942,58 +921,58 @@
         <v>2022</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2">
-        <v>0.18892489619187439</v>
+        <v>4.6740245270914631E-2</v>
       </c>
       <c r="G2">
-        <v>0.75901393082335944</v>
+        <v>0.1559226316027181</v>
       </c>
       <c r="H2">
-        <v>1.85390797856095</v>
+        <v>0.38084440749714182</v>
       </c>
       <c r="I2">
         <v>0.35327920470807511</v>
       </c>
       <c r="J2">
-        <v>0.53477502687424949</v>
+        <v>0.1323039812364202</v>
       </c>
       <c r="K2">
         <v>2.9436944270154521</v>
       </c>
       <c r="L2">
-        <v>4.0175431937381916</v>
+        <v>3.3359395248990089</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>380000</v>
       </c>
       <c r="N2">
         <v>14308576.598999999</v>
       </c>
       <c r="O2">
-        <v>8.3688165910542012E-2</v>
+        <v>14.65405145143866</v>
       </c>
       <c r="P2">
-        <v>156018.96900000001</v>
+        <v>176339.81299999999</v>
       </c>
       <c r="Q2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1001,37 +980,37 @@
         <v>2022</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3">
-        <v>0.1154433422751292</v>
+        <v>0.13975741390730839</v>
       </c>
       <c r="G3">
-        <v>3.085611380353208E-3</v>
+        <v>1.4709910084041391</v>
       </c>
       <c r="H3">
-        <v>7.5366726807897817E-3</v>
+        <v>3.592927423497458</v>
       </c>
       <c r="I3">
         <v>0.27664423601485799</v>
       </c>
       <c r="J3">
-        <v>0.41729892492294313</v>
+        <v>0.5051882371400731</v>
       </c>
       <c r="K3">
         <v>4.3818587553913364</v>
       </c>
       <c r="L3">
-        <v>2.6728361458900379E-2</v>
+        <v>10.525316455696199</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1040,19 +1019,19 @@
         <v>66488.866999999998</v>
       </c>
       <c r="O3">
-        <v>7.6657812508344643</v>
+        <v>1.5216030165553091E-3</v>
       </c>
       <c r="P3">
-        <v>18.37</v>
+        <v>0.158</v>
       </c>
       <c r="Q3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1060,55 +1039,58 @@
         <v>2022</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="F4">
-        <v>0.1896616223840121</v>
+        <v>0.1345330182718662</v>
       </c>
       <c r="G4">
-        <v>9.6756901800207976E-2</v>
+        <v>7.9826881068388822</v>
       </c>
       <c r="H4">
-        <v>0.2363308299673218</v>
+        <v>19.49788873516253</v>
       </c>
       <c r="I4">
-        <v>0.33491753091626458</v>
+        <v>0.39323711430581693</v>
       </c>
       <c r="J4">
-        <v>0.56629350474768336</v>
+        <v>0.3421167874994655</v>
       </c>
       <c r="K4">
-        <v>0.47567893708967901</v>
+        <v>5.7168616229301286</v>
       </c>
       <c r="L4">
-        <v>0.51015540510510948</v>
+        <v>59.336274539736813</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1079682.5819999999</v>
+        <v>4178.8860000000004</v>
       </c>
       <c r="O4">
-        <v>38.224789649248123</v>
+        <v>2.2316844242811201E-2</v>
       </c>
       <c r="P4">
-        <v>67.501000000000005</v>
+        <v>32.753</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>133</v>
       </c>
       <c r="R4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1116,58 +1098,55 @@
         <v>2022</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="F5">
-        <v>6.1521978842644112E-2</v>
+        <v>0.22606461177078191</v>
       </c>
       <c r="G5">
-        <v>2.138365134366112E-2</v>
+        <v>3.4111570282362429</v>
       </c>
       <c r="H5">
-        <v>5.223003192283289E-2</v>
+        <v>8.3318249823311472</v>
       </c>
       <c r="I5">
-        <v>0.15137432579459439</v>
+        <v>0.33491753091626458</v>
       </c>
       <c r="J5">
-        <v>0.40642280994285412</v>
+        <v>0.67498590220797405</v>
       </c>
       <c r="K5">
-        <v>0.15642017049486759</v>
+        <v>0.47567893708967901</v>
       </c>
       <c r="L5">
-        <v>0.34757743079679659</v>
+        <v>15.08930124673819</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>5904311.2220000001</v>
+        <v>1079682.5819999999</v>
       </c>
       <c r="O5">
-        <v>1.014402011036873E-3</v>
+        <v>8.7826679944992062E-3</v>
       </c>
       <c r="P5">
-        <v>4648.9900000000007</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>124</v>
+        <v>3.4489999999999998</v>
       </c>
       <c r="R5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1175,58 +1154,58 @@
         <v>2022</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6">
-        <v>7.9409505863521038E-2</v>
+        <v>7.6038261281544131E-2</v>
       </c>
       <c r="G6">
-        <v>4.2900535412027539E-3</v>
+        <v>2.6810241438290219E-2</v>
       </c>
       <c r="H6">
-        <v>1.047854876637354E-2</v>
+        <v>6.5484595856724642E-2</v>
       </c>
       <c r="I6">
-        <v>0.1834237992556193</v>
+        <v>0.15137432579459439</v>
       </c>
       <c r="J6">
-        <v>0.4329291301662333</v>
+        <v>0.50231940510653939</v>
       </c>
       <c r="K6">
-        <v>5.8305191328575118E-2</v>
+        <v>0.15642017049486759</v>
       </c>
       <c r="L6">
-        <v>5.402443315257436E-2</v>
+        <v>0.35258882812983983</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>152809177.19299999</v>
+        <v>5904311.2220000001</v>
       </c>
       <c r="O6">
-        <v>1.8522202860116961</v>
+        <v>2.2605948815956709</v>
       </c>
       <c r="P6">
-        <v>17268.668000000001</v>
+        <v>18918.444</v>
       </c>
       <c r="Q6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="R6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1234,55 +1213,55 @@
         <v>2022</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7">
-        <v>5.0004609063333462E-2</v>
+        <v>8.0419027328200041E-2</v>
       </c>
       <c r="G7">
-        <v>2.2029661612112231E-2</v>
+        <v>1.5917330291396681E-2</v>
       </c>
       <c r="H7">
-        <v>5.3807926006561542E-2</v>
+        <v>3.8878424263701299E-2</v>
       </c>
       <c r="I7">
-        <v>0.13136127287689589</v>
+        <v>0.1834237992556193</v>
       </c>
       <c r="J7">
-        <v>0.38066477256348491</v>
+        <v>0.43843289504721328</v>
       </c>
       <c r="K7">
-        <v>0.19149461828593969</v>
+        <v>5.8305191328575118E-2</v>
       </c>
       <c r="L7">
-        <v>0.44055262154355629</v>
+        <v>0.1979299031613013</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>118000</v>
       </c>
       <c r="N7">
-        <v>6255187.0319999997</v>
+        <v>152809177.19299999</v>
       </c>
       <c r="O7">
-        <v>28.686781671117242</v>
+        <v>1.369442714899778E-2</v>
       </c>
       <c r="P7">
-        <v>10502.305</v>
+        <v>309651.31099999999</v>
       </c>
       <c r="R7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1290,58 +1269,55 @@
         <v>2022</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="F8">
-        <v>0.1916465924644388</v>
+        <v>5.6836361347521833E-2</v>
       </c>
       <c r="G8">
-        <v>7.5048805609074218</v>
+        <v>1.7043735709023851E-2</v>
       </c>
       <c r="H8">
-        <v>18.33083344718111</v>
+        <v>4.1629693912425693E-2</v>
       </c>
       <c r="I8">
-        <v>0.48520186844616309</v>
+        <v>0.13136127287689589</v>
       </c>
       <c r="J8">
-        <v>0.39498321199417108</v>
+        <v>0.43267212704908498</v>
       </c>
       <c r="K8">
-        <v>20.37978068563628</v>
+        <v>0.19149461828593969</v>
       </c>
       <c r="L8">
-        <v>39.159999999999997</v>
+        <v>0.29987380094251931</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>36000</v>
       </c>
       <c r="N8">
-        <v>914.30399999999997</v>
+        <v>6255187.0319999997</v>
       </c>
       <c r="O8">
-        <v>6.4098188996315007E-3</v>
+        <v>187.39301950386911</v>
       </c>
       <c r="P8">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>118</v>
+        <v>153814.144</v>
       </c>
       <c r="R8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1349,58 +1325,58 @@
         <v>2022</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="F9">
-        <v>0.2714911262046108</v>
+        <v>0.20700452772892169</v>
       </c>
       <c r="G9">
-        <v>5.3710656921956126</v>
+        <v>13.82903471186691</v>
       </c>
       <c r="H9">
-        <v>13.11894437739085</v>
+        <v>33.777717044422623</v>
       </c>
       <c r="I9">
-        <v>0.57113303042337438</v>
+        <v>0.48520186844616309</v>
       </c>
       <c r="J9">
-        <v>0.47535532309058981</v>
+        <v>0.42663588331150548</v>
       </c>
       <c r="K9">
-        <v>11.068200120028729</v>
+        <v>20.37978068563628</v>
       </c>
       <c r="L9">
-        <v>19.783577339274359</v>
+        <v>66.805469733379098</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>12050.448</v>
+        <v>914.30399999999997</v>
       </c>
       <c r="O9">
-        <v>3.1446462342143058E-2</v>
+        <v>1.3481402726680041</v>
       </c>
       <c r="P9">
-        <v>10.997</v>
+        <v>8.7390000000000008</v>
       </c>
       <c r="Q9" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="R9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1408,58 +1384,58 @@
         <v>2022</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="F10">
-        <v>0.12547094149077001</v>
+        <v>0.2134034585984928</v>
       </c>
       <c r="G10">
-        <v>0.61180963505676345</v>
+        <v>3.4605991612445339</v>
       </c>
       <c r="H10">
-        <v>1.49435829532378</v>
+        <v>8.452588463920625</v>
       </c>
       <c r="I10">
-        <v>0.29847521717046888</v>
+        <v>0.57113303042337438</v>
       </c>
       <c r="J10">
-        <v>0.42037306373449912</v>
+        <v>0.37364930275578567</v>
       </c>
       <c r="K10">
-        <v>0.38012845711234378</v>
+        <v>11.068200120028729</v>
       </c>
       <c r="L10">
-        <v>4.8761061946902657</v>
+        <v>16.216228096637678</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1249404.5449999999</v>
+        <v>12050.448</v>
       </c>
       <c r="O10">
-        <v>3.1858785152435301E-2</v>
+        <v>1.2806825389340519</v>
       </c>
       <c r="P10">
-        <v>0.33900000000000002</v>
+        <v>116.021</v>
       </c>
       <c r="Q10" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="R10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1467,58 +1443,58 @@
         <v>2022</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="F11">
-        <v>8.5885986776801343E-2</v>
+        <v>9.531301391558708E-2</v>
       </c>
       <c r="G11">
-        <v>0.66681293290025689</v>
+        <v>6.1650124445294649E-2</v>
       </c>
       <c r="H11">
-        <v>1.6287050425680649</v>
+        <v>0.15058176529701409</v>
       </c>
       <c r="I11">
-        <v>0.19454830922947361</v>
+        <v>0.29847521717046888</v>
       </c>
       <c r="J11">
-        <v>0.44146354762454959</v>
+        <v>0.31933309176939367</v>
       </c>
       <c r="K11">
-        <v>2.6269272230522791</v>
+        <v>0.38012845711234378</v>
       </c>
       <c r="L11">
-        <v>7.7639316718006164</v>
+        <v>0.64681749021066948</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>24070.644</v>
+        <v>1249404.5449999999</v>
       </c>
       <c r="O11">
-        <v>7.9842436313629149E-4</v>
+        <v>14.15946006774902</v>
       </c>
       <c r="P11">
-        <v>3.5710000000000002</v>
+        <v>4450.7640000000001</v>
       </c>
       <c r="Q11" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="R11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1526,58 +1502,58 @@
         <v>2022</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F12">
-        <v>0.1652902826489431</v>
+        <v>0.1091694010873582</v>
       </c>
       <c r="G12">
-        <v>8.4065334212879927E-2</v>
+        <v>0.64996854406916615</v>
       </c>
       <c r="H12">
-        <v>0.20533140103053099</v>
+        <v>1.58756225772607</v>
       </c>
       <c r="I12">
-        <v>0.30701408640608763</v>
+        <v>0.19454830922947361</v>
       </c>
       <c r="J12">
-        <v>0.53838012640994459</v>
+        <v>0.56114289309289622</v>
       </c>
       <c r="K12">
-        <v>0.24846427096055021</v>
+        <v>2.6269272230522791</v>
       </c>
       <c r="L12">
-        <v>0.5085921136176208</v>
+        <v>5.9537611967757904</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
-        <v>18410088.155999999</v>
+        <v>24070.644</v>
       </c>
       <c r="O12">
-        <v>0.32283568954467767</v>
+        <v>0.60001878952831023</v>
       </c>
       <c r="P12">
-        <v>685.1049999999999</v>
+        <v>347.86799999999988</v>
       </c>
       <c r="Q12" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="R12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1585,58 +1561,58 @@
         <v>2022</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="F13">
-        <v>0.42041134541060121</v>
+        <v>0.14602482676535539</v>
       </c>
       <c r="G13">
-        <v>9.3402216920406769</v>
+        <v>5.0646167979102492E-2</v>
       </c>
       <c r="H13">
-        <v>22.813693943164392</v>
+        <v>0.1237043631045652</v>
       </c>
       <c r="I13">
-        <v>0.49289711580487661</v>
+        <v>0.30701408640608763</v>
       </c>
       <c r="J13">
-        <v>0.85293934967359308</v>
+        <v>0.47562907772319057</v>
       </c>
       <c r="K13">
-        <v>20.844300865026121</v>
+        <v>0.24846427096055021</v>
       </c>
       <c r="L13">
-        <v>22.216864016641619</v>
+        <v>0.34683258388989491</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>536856.27100000007</v>
+        <v>18410088.155999999</v>
       </c>
       <c r="O13">
-        <v>15.64106770164072</v>
+        <v>0.2435194307565689</v>
       </c>
       <c r="P13">
-        <v>1015.2859999999999</v>
+        <v>12263.545</v>
       </c>
       <c r="Q13" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="R13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1644,58 +1620,58 @@
         <v>2022</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F14">
-        <v>0.18705479535339811</v>
+        <v>0.1534871328660305</v>
       </c>
       <c r="G14">
-        <v>3.8265160929176339E-3</v>
+        <v>8.3372901811330369</v>
       </c>
       <c r="H14">
-        <v>9.3463485012145603E-3</v>
+        <v>20.364011988045469</v>
       </c>
       <c r="I14">
-        <v>0.32727999884289088</v>
+        <v>0.49289711580487661</v>
       </c>
       <c r="J14">
-        <v>0.5715436201868016</v>
+        <v>0.31139791235214193</v>
       </c>
       <c r="K14">
-        <v>0.23023404203322509</v>
+        <v>20.844300865026121</v>
       </c>
       <c r="L14">
-        <v>2.0456658626090231E-2</v>
+        <v>54.319147315170362</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
-        <v>785933423.98899996</v>
+        <v>536856.27100000007</v>
       </c>
       <c r="O14">
-        <v>3.1717190551757821</v>
+        <v>1.6788112454772</v>
       </c>
       <c r="P14">
-        <v>2514522.872</v>
+        <v>65.628</v>
       </c>
       <c r="Q14" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="R14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1703,58 +1679,58 @@
         <v>2022</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F15">
-        <v>6.48546606342945E-2</v>
+        <v>0.15824636197155539</v>
       </c>
       <c r="G15">
-        <v>0.11155358477610899</v>
+        <v>5.2869459730133843E-2</v>
       </c>
       <c r="H15">
-        <v>0.27247204887156862</v>
+        <v>0.12913480139893829</v>
       </c>
       <c r="I15">
-        <v>0.1036844199247966</v>
+        <v>0.32727999884289088</v>
       </c>
       <c r="J15">
-        <v>0.62550053982396081</v>
+        <v>0.48351980729357302</v>
       </c>
       <c r="K15">
-        <v>2.7301398234800032</v>
+        <v>0.23023404203322509</v>
       </c>
       <c r="L15">
-        <v>1.7200550228015621</v>
+        <v>0.3340958937156297</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>33504797.620000001</v>
+        <v>785933423.98899996</v>
       </c>
       <c r="O15">
-        <v>6690.1733524412812</v>
+        <v>674240.75114424329</v>
       </c>
       <c r="P15">
-        <v>141888.08600000001</v>
+        <v>6766640.9809999987</v>
       </c>
       <c r="Q15" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="R15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1762,58 +1738,58 @@
         <v>2022</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="F16">
-        <v>6.4463115877142596E-2</v>
+        <v>4.6450938619667398E-2</v>
       </c>
       <c r="G16">
-        <v>5.2070738146694377E-2</v>
+        <v>6.0830837466893432E-2</v>
       </c>
       <c r="H16">
-        <v>0.1271839066181521</v>
+        <v>0.14858063909325461</v>
       </c>
       <c r="I16">
-        <v>0.15162522238314771</v>
+        <v>0.1036844199247966</v>
       </c>
       <c r="J16">
-        <v>0.42514770869880902</v>
+        <v>0.44800307175715282</v>
       </c>
       <c r="K16">
-        <v>0.61770899001935942</v>
+        <v>2.7301398234800032</v>
       </c>
       <c r="L16">
-        <v>0.80776018096819424</v>
+        <v>1.3095717605400019</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>415438.26</v>
+        <v>33504797.620000001</v>
       </c>
       <c r="O16">
-        <v>67.919793849979342</v>
+        <v>2.4838601112365719E-2</v>
       </c>
       <c r="P16">
-        <v>3317.268</v>
+        <v>45.185000000000002</v>
       </c>
       <c r="Q16" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="R16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1821,58 +1797,58 @@
         <v>2022</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F17">
-        <v>6.9169079483441712E-2</v>
+        <v>1.3005709033249919E-2</v>
       </c>
       <c r="G17">
-        <v>7.9727248454161456E-3</v>
+        <v>5.783654990151022E-3</v>
       </c>
       <c r="H17">
-        <v>1.9473553253172019E-2</v>
+        <v>1.4126702681008079E-2</v>
       </c>
       <c r="I17">
-        <v>0.2006637721006648</v>
+        <v>0.15162522238314771</v>
       </c>
       <c r="J17">
-        <v>0.34470138161632102</v>
+        <v>8.5775366583702634E-2</v>
       </c>
       <c r="K17">
-        <v>7.8723177732298935E-2</v>
+        <v>0.61770899001935942</v>
       </c>
       <c r="L17">
-        <v>0.1152642901272775</v>
+        <v>0.4447012443046926</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="N17">
-        <v>10230673.141000001</v>
+        <v>415438.26</v>
       </c>
       <c r="O17">
-        <v>145.59935059593909</v>
+        <v>4.5435066074341526</v>
       </c>
       <c r="P17">
-        <v>3505.8820000000001</v>
+        <v>15101.687</v>
       </c>
       <c r="Q17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1880,58 +1856,58 @@
         <v>2022</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F18">
-        <v>0.1607502127186887</v>
+        <v>1.186195631861698E-2</v>
       </c>
       <c r="G18">
-        <v>9.5023941035404721E-2</v>
+        <v>1.310169056880459E-3</v>
       </c>
       <c r="H18">
-        <v>0.23209803573531521</v>
+        <v>3.2001163208948131E-3</v>
       </c>
       <c r="I18">
-        <v>0.42615798826202128</v>
+        <v>0.2006637721006648</v>
       </c>
       <c r="J18">
-        <v>0.37720802412801929</v>
+        <v>5.9113591827957473E-2</v>
       </c>
       <c r="K18">
-        <v>0.45939474624123788</v>
+        <v>7.8723177732298935E-2</v>
       </c>
       <c r="L18">
-        <v>0.5911279333838001</v>
+        <v>0.1104513472895014</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="N18">
-        <v>1391186.602</v>
+        <v>10230673.141000001</v>
       </c>
       <c r="O18">
-        <v>24.885179257392881</v>
+        <v>9.6210135757923129E-2</v>
       </c>
       <c r="P18">
-        <v>66.05</v>
+        <v>82021.606999999989</v>
       </c>
       <c r="Q18" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="R18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -1939,58 +1915,58 @@
         <v>2022</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="F19">
-        <v>3.2009270922853612E-2</v>
+        <v>0.17445527607454239</v>
       </c>
       <c r="G19">
-        <v>93.4522945264942</v>
+        <v>7.8772188757020176E-2</v>
       </c>
       <c r="H19">
-        <v>228.2592550700038</v>
+        <v>0.19240277851940379</v>
       </c>
       <c r="I19">
-        <v>4.9356777146401458E-2</v>
+        <v>0.42615798826202128</v>
       </c>
       <c r="J19">
-        <v>0.64852838401316415</v>
+        <v>0.40936760750634887</v>
       </c>
       <c r="K19">
-        <v>217.37724697042279</v>
+        <v>0.45939474624123788</v>
       </c>
       <c r="L19">
-        <v>2919.5383659854679</v>
+        <v>0.45153228110660232</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
-        <v>1836490.629</v>
+        <v>1391186.602</v>
       </c>
       <c r="O19">
-        <v>40.383367074170707</v>
+        <v>91.756923872530464</v>
       </c>
       <c r="P19">
-        <v>21012.101999999999</v>
+        <v>7685.7960000000012</v>
       </c>
       <c r="Q19" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="R19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1998,58 +1974,58 @@
         <v>2022</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F20">
-        <v>0.25404014610076531</v>
+        <v>2.1652013887886901E-2</v>
       </c>
       <c r="G20">
-        <v>0.44188053191401327</v>
+        <v>815.66088213897001</v>
       </c>
       <c r="H20">
-        <v>1.0793027774832691</v>
+        <v>1992.269385039014</v>
       </c>
       <c r="I20">
-        <v>0.470663478647389</v>
+        <v>4.9356777146401458E-2</v>
       </c>
       <c r="J20">
-        <v>0.53974900884775623</v>
+        <v>0.43868370545473351</v>
       </c>
       <c r="K20">
-        <v>1.2418337582312671</v>
+        <v>217.37724697042279</v>
       </c>
       <c r="L20">
-        <v>1.7394122098274221</v>
+        <v>37671.363336566443</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
-        <v>719464.15700000001</v>
+        <v>1836490.629</v>
       </c>
       <c r="O20">
-        <v>3.398270416259766E-2</v>
+        <v>1.04005753993988E-3</v>
       </c>
       <c r="P20">
-        <v>81.934000000000012</v>
+        <v>10.31</v>
       </c>
       <c r="Q20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="R20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -2057,58 +2033,58 @@
         <v>2022</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F21">
-        <v>7.6444397145136291E-3</v>
+        <v>0.1631015313221649</v>
       </c>
       <c r="G21">
-        <v>2.9736931228700362E-4</v>
+        <v>0.90717108832089222</v>
       </c>
       <c r="H21">
-        <v>7.2633099109265008E-4</v>
+        <v>2.2157850472303391</v>
       </c>
       <c r="I21">
-        <v>7.0392923645923547E-2</v>
+        <v>0.470663478647389</v>
       </c>
       <c r="J21">
-        <v>0.1085967071486499</v>
+        <v>0.34653534578653178</v>
       </c>
       <c r="K21">
-        <v>3.4034530676471053E-2</v>
+        <v>1.2418337582312671</v>
       </c>
       <c r="L21">
-        <v>3.8900079455453387E-2</v>
+        <v>5.5620022753128557</v>
       </c>
       <c r="M21">
-        <v>330000</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>37269351.472999997</v>
+        <v>719464.15700000001</v>
       </c>
       <c r="O21">
-        <v>1.594639961349964</v>
+        <v>1.9842205166816711E-3</v>
       </c>
       <c r="P21">
-        <v>133473.53200000001</v>
+        <v>0.87900000000000011</v>
       </c>
       <c r="Q21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R21" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -2116,58 +2092,58 @@
         <v>2022</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F22">
-        <v>9.7654749940174868E-2</v>
+        <v>3.4962425798088221E-3</v>
       </c>
       <c r="G22">
-        <v>5.8505348187650654E-3</v>
+        <v>1.9540458807658061E-4</v>
       </c>
       <c r="H22">
-        <v>1.4290058112097289E-2</v>
+        <v>4.772799420026663E-4</v>
       </c>
       <c r="I22">
-        <v>0.2025218362484637</v>
+        <v>7.0392923645923547E-2</v>
       </c>
       <c r="J22">
-        <v>0.48219368216851061</v>
+        <v>4.9667529045887122E-2</v>
       </c>
       <c r="K22">
-        <v>0.1086791112874493</v>
+        <v>3.4034530676471053E-2</v>
       </c>
       <c r="L22">
-        <v>5.9910396804550861E-2</v>
+        <v>5.5889882814500122E-2</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>2410284</v>
       </c>
       <c r="N22">
-        <v>1612945510.7279999</v>
+        <v>37269351.472999997</v>
       </c>
       <c r="O22">
-        <v>0.21239190101623531</v>
+        <v>36.020908210913838</v>
       </c>
       <c r="P22">
-        <v>859486.31199999992</v>
+        <v>329100.52899999998</v>
       </c>
       <c r="Q22" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="R22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -2175,58 +2151,58 @@
         <v>2022</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="F23">
-        <v>9.0050536529963476E-2</v>
+        <v>0.114212485923084</v>
       </c>
       <c r="G23">
-        <v>2.6362272962046601E-2</v>
+        <v>1.305364260710901E-2</v>
       </c>
       <c r="H23">
-        <v>6.4390423143252912E-2</v>
+        <v>3.1883805021010257E-2</v>
       </c>
       <c r="I23">
-        <v>0.10187742563033229</v>
+        <v>0.2025218362484637</v>
       </c>
       <c r="J23">
-        <v>0.88391060112489162</v>
+        <v>0.56395146340151925</v>
       </c>
       <c r="K23">
-        <v>0.1635366634742359</v>
+        <v>0.1086791112874493</v>
       </c>
       <c r="L23">
-        <v>0.29274976005584152</v>
+        <v>0.1142926055904251</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23">
-        <v>19662149.114999998</v>
+        <v>1612945510.7279999</v>
       </c>
       <c r="O23">
-        <v>1.058416986465454E-2</v>
+        <v>293931.2363798967</v>
       </c>
       <c r="P23">
-        <v>4584.3999999999996</v>
+        <v>3010729.9</v>
       </c>
       <c r="Q23" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="R23" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -2234,58 +2210,58 @@
         <v>2022</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F24">
-        <v>0.1248565508088034</v>
+        <v>4.4342286691684312E-5</v>
       </c>
       <c r="G24">
-        <v>0.1226607416646479</v>
+        <v>3.2179033815737989E-5</v>
       </c>
       <c r="H24">
-        <v>0.29960152033259069</v>
+        <v>7.8597987613567092E-5</v>
       </c>
       <c r="I24">
-        <v>0.20162261443817811</v>
+        <v>0.10187742563033229</v>
       </c>
       <c r="J24">
-        <v>0.61925866379977512</v>
+        <v>4.3525134657978771E-4</v>
       </c>
       <c r="K24">
-        <v>2.1514467153937882</v>
+        <v>0.1635366634742359</v>
       </c>
       <c r="L24">
-        <v>0.98241334451471407</v>
+        <v>0.72569630969826937</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>290000</v>
       </c>
       <c r="N24">
-        <v>3038719.1349999998</v>
+        <v>19662149.114999998</v>
       </c>
       <c r="O24">
-        <v>2397.7065828543659</v>
+        <v>6.1942642882466311E-3</v>
       </c>
       <c r="P24">
-        <v>3871.913</v>
+        <v>465.38200000000001</v>
       </c>
       <c r="Q24" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="R24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -2293,58 +2269,58 @@
         <v>2022</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F25">
-        <v>3.6048632409209178E-2</v>
+        <v>8.9500167237576853E-2</v>
       </c>
       <c r="G25">
-        <v>2.411261696562603E-2</v>
+        <v>0.41981961889593722</v>
       </c>
       <c r="H25">
-        <v>5.8895589608040512E-2</v>
+        <v>1.0254185192402301</v>
       </c>
       <c r="I25">
-        <v>8.8022234465224586E-2</v>
+        <v>0.20162261443817811</v>
       </c>
       <c r="J25">
-        <v>0.40954007391679098</v>
+        <v>0.44389944792140151</v>
       </c>
       <c r="K25">
-        <v>9.2157292517239531E-2</v>
+        <v>2.1514467153937882</v>
       </c>
       <c r="L25">
-        <v>0.66889131026968129</v>
+        <v>4.6907132338818123</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25">
-        <v>130667741.07700001</v>
+        <v>3038719.1349999998</v>
       </c>
       <c r="O25">
-        <v>3.4996869380772122E-2</v>
+        <v>3.043206033110619E-3</v>
       </c>
       <c r="P25">
-        <v>7.3419999999999996</v>
+        <v>62.475999999999999</v>
       </c>
       <c r="Q25" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="R25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -2352,58 +2328,58 @@
         <v>2022</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E26" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F26">
-        <v>0.18471670330761139</v>
+        <v>3.8185625092489003E-2</v>
       </c>
       <c r="G26">
-        <v>7.4297579635770781</v>
+        <v>5.7599676142629742E-3</v>
       </c>
       <c r="H26">
-        <v>18.14734487483058</v>
+        <v>1.4068845751949629E-2</v>
       </c>
       <c r="I26">
-        <v>0.31981095428556261</v>
+        <v>8.8022234465224586E-2</v>
       </c>
       <c r="J26">
-        <v>0.5775809140754945</v>
+        <v>0.43381794752751018</v>
       </c>
       <c r="K26">
-        <v>38.888626413191282</v>
+        <v>9.2157292517239531E-2</v>
       </c>
       <c r="L26">
-        <v>40.22244783788824</v>
+        <v>0.15084125506160539</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26">
-        <v>405775.13299999997</v>
+        <v>130667741.07700001</v>
       </c>
       <c r="O26">
-        <v>9.5842616558074949E-4</v>
+        <v>266.22553594875342</v>
       </c>
       <c r="P26">
-        <v>48.262999999999998</v>
+        <v>738.89599999999996</v>
       </c>
       <c r="Q26" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="R26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -2411,58 +2387,58 @@
         <v>2022</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="F27">
-        <v>0.18679547838228269</v>
+        <v>0.1568550415914074</v>
       </c>
       <c r="G27">
-        <v>0.13659617416624861</v>
+        <v>5.6924068113282571</v>
       </c>
       <c r="H27">
-        <v>0.33363911628473603</v>
+        <v>13.903827026321251</v>
       </c>
       <c r="I27">
-        <v>0.42040077556916239</v>
+        <v>0.31981095428556261</v>
       </c>
       <c r="J27">
-        <v>0.44432714979982701</v>
+        <v>0.49046175401280928</v>
       </c>
       <c r="K27">
-        <v>5.8301617279052177E-2</v>
+        <v>38.888626413191282</v>
       </c>
       <c r="L27">
-        <v>0.73126060303612028</v>
+        <v>36.290875661851153</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27">
-        <v>2611109.0070000002</v>
+        <v>405775.13299999997</v>
       </c>
       <c r="O27">
-        <v>0.2207643364071846</v>
+        <v>6.6563682556152345E-2</v>
       </c>
       <c r="P27">
-        <v>797.53099999999995</v>
+        <v>339.38900000000001</v>
       </c>
       <c r="Q27" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="R27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2470,58 +2446,58 @@
         <v>2022</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F28">
-        <v>8.6824364275404409E-2</v>
+        <v>0.18667318687598891</v>
       </c>
       <c r="G28">
-        <v>6.671591807131913E-2</v>
+        <v>3.1759053909797781E-2</v>
       </c>
       <c r="H28">
-        <v>0.16295507603564879</v>
+        <v>7.7572177589746827E-2</v>
       </c>
       <c r="I28">
-        <v>0.20351833729028621</v>
+        <v>0.42040077556916239</v>
       </c>
       <c r="J28">
-        <v>0.4266169104534468</v>
+        <v>0.44403625712455008</v>
       </c>
       <c r="K28">
-        <v>0.1810664701390482</v>
+        <v>5.8301617279052177E-2</v>
       </c>
       <c r="L28">
-        <v>0.76840088180430721</v>
+        <v>0.17013184614936699</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28">
-        <v>45346298.25</v>
+        <v>2611109.0070000002</v>
       </c>
       <c r="O28">
-        <v>2.7944852709770198</v>
+        <v>0.3317094576090574</v>
       </c>
       <c r="P28">
-        <v>294.85000000000002</v>
+        <v>6594.6559999999999</v>
       </c>
       <c r="Q28" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="R28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2529,58 +2505,58 @@
         <v>2022</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="E29" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="F29">
-        <v>0.2016852850610428</v>
+        <v>0.111679028387435</v>
       </c>
       <c r="G29">
-        <v>0.2562773045168974</v>
+        <v>2.7070541870628542E-2</v>
       </c>
       <c r="H29">
-        <v>0.6259628713962837</v>
+        <v>6.6120385305030796E-2</v>
       </c>
       <c r="I29">
-        <v>0.49775437404450479</v>
+        <v>0.20351833729028621</v>
       </c>
       <c r="J29">
-        <v>0.40519038220045839</v>
+        <v>0.54874184741467702</v>
       </c>
       <c r="K29">
-        <v>21.13944423742846</v>
+        <v>0.1810664701390482</v>
       </c>
       <c r="L29">
-        <v>1.270679238891085</v>
+        <v>0.24239592931195519</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
       <c r="N29">
-        <v>1924.1669999999999</v>
+        <v>45346298.25</v>
       </c>
       <c r="O29">
-        <v>5.7294932298660282</v>
+        <v>9.5508408069610612E-2</v>
       </c>
       <c r="P29">
-        <v>17.710999999999999</v>
+        <v>505103.8</v>
       </c>
       <c r="Q29" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="R29" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -2588,58 +2564,58 @@
         <v>2022</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E30" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="F30">
-        <v>0.11080024523663019</v>
+        <v>0.23151112702156229</v>
       </c>
       <c r="G30">
-        <v>1.6008953783318729</v>
+        <v>16.092519404839791</v>
       </c>
       <c r="H30">
-        <v>3.9102216628768489</v>
+        <v>39.306327470717378</v>
       </c>
       <c r="I30">
-        <v>0.2326102658434335</v>
+        <v>0.49775437404450479</v>
       </c>
       <c r="J30">
-        <v>0.4763342874609332</v>
+        <v>0.4651111855440222</v>
       </c>
       <c r="K30">
-        <v>19.257776430756518</v>
+        <v>21.13944423742846</v>
       </c>
       <c r="L30">
-        <v>14.44848226565678</v>
+        <v>69.510781671159052</v>
       </c>
       <c r="M30">
         <v>0</v>
       </c>
       <c r="N30">
-        <v>150778.78099999999</v>
+        <v>1924.1669999999999</v>
       </c>
       <c r="O30">
-        <v>1.420162815451622E-2</v>
+        <v>1.2680025137960909E-2</v>
       </c>
       <c r="P30">
-        <v>51.622999999999998</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="Q30" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="R30" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -2647,58 +2623,58 @@
         <v>2022</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="F31">
-        <v>4.5376626236371967E-2</v>
+        <v>9.6071970833123702E-2</v>
       </c>
       <c r="G31">
-        <v>0.1241891789414143</v>
+        <v>2.9037350735434311</v>
       </c>
       <c r="H31">
-        <v>0.30333476151177879</v>
+        <v>7.0924358590227854</v>
       </c>
       <c r="I31">
-        <v>0.10381906119690559</v>
+        <v>0.2326102658434335</v>
       </c>
       <c r="J31">
-        <v>0.43707413372106713</v>
+        <v>0.41301689968313049</v>
       </c>
       <c r="K31">
-        <v>1.136467976927054</v>
+        <v>19.257776430756518</v>
       </c>
       <c r="L31">
-        <v>2.7368535134035499</v>
+        <v>30.22458109646983</v>
       </c>
       <c r="M31">
         <v>0</v>
       </c>
       <c r="N31">
-        <v>691642364.98099995</v>
+        <v>150778.78099999999</v>
       </c>
       <c r="O31">
-        <v>2.028804022073746E-3</v>
+        <v>3.550407038629055E-3</v>
       </c>
       <c r="P31">
-        <v>61705.706999999988</v>
+        <v>12.294</v>
       </c>
       <c r="Q31" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="R31" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2706,58 +2682,58 @@
         <v>2022</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="E32" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="F32">
-        <v>0.13139408379285661</v>
+        <v>5.635052620900937E-2</v>
       </c>
       <c r="G32">
-        <v>0.4183893970678294</v>
+        <v>5.1653685569322663E-2</v>
       </c>
       <c r="H32">
-        <v>1.021925171423326</v>
+        <v>0.1261652466578137</v>
       </c>
       <c r="I32">
-        <v>0.26749007657640972</v>
+        <v>0.10381906119690559</v>
       </c>
       <c r="J32">
-        <v>0.49121105902156081</v>
+        <v>0.54277630291930379</v>
       </c>
       <c r="K32">
-        <v>0.102481222268647</v>
+        <v>1.136467976927054</v>
       </c>
       <c r="L32">
-        <v>3.1842331480268351</v>
+        <v>0.91664956912264339</v>
       </c>
       <c r="M32">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N32">
-        <v>48269781.395000003</v>
+        <v>691642364.98099995</v>
       </c>
       <c r="O32">
-        <v>17576.652826826808</v>
+        <v>6642641.0442392984</v>
       </c>
       <c r="P32">
-        <v>39093.79</v>
+        <v>26398401.59</v>
       </c>
       <c r="Q32" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="R32" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -2765,58 +2741,58 @@
         <v>2022</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F33">
-        <v>0.39473563740053619</v>
+        <v>0.14230720093306079</v>
       </c>
       <c r="G33">
-        <v>3.1874295184270558</v>
+        <v>1.3200792491222451</v>
       </c>
       <c r="H33">
-        <v>7.7853656900637542</v>
+        <v>3.2243221802605162</v>
       </c>
       <c r="I33">
-        <v>0.86928621834781017</v>
+        <v>0.26749007657640972</v>
       </c>
       <c r="J33">
-        <v>0.45409167782595461</v>
+        <v>0.53200927209877324</v>
       </c>
       <c r="K33">
-        <v>25.969812776686499</v>
+        <v>0.102481222268647</v>
       </c>
       <c r="L33">
-        <v>8.0748460904551855</v>
+        <v>9.2762645914396895</v>
       </c>
       <c r="M33">
         <v>0</v>
       </c>
       <c r="N33">
-        <v>121185.442</v>
+        <v>48269781.395000003</v>
       </c>
       <c r="O33">
-        <v>1.0306535875797269</v>
+        <v>5.0720100551843639E-4</v>
       </c>
       <c r="P33">
-        <v>41.258000000000003</v>
+        <v>1.2849999999999999</v>
       </c>
       <c r="Q33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R33" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -2824,58 +2800,58 @@
         <v>2022</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F34">
-        <v>0.13342541984893019</v>
+        <v>0.31032522175104738</v>
       </c>
       <c r="G34">
-        <v>7046.1256319950025</v>
+        <v>7.8094612551981744</v>
       </c>
       <c r="H34">
-        <v>17210.314589256719</v>
+        <v>19.074778395133151</v>
       </c>
       <c r="I34">
-        <v>0.3236120898438461</v>
+        <v>0.86928621834781017</v>
       </c>
       <c r="J34">
-        <v>0.41230047960603849</v>
+        <v>0.35698854439549288</v>
       </c>
       <c r="K34">
-        <v>58808.860480769821</v>
+        <v>25.969812776686499</v>
       </c>
       <c r="L34">
-        <v>52809.469439728353</v>
+        <v>25.165409408659571</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
       <c r="N34">
-        <v>491.75299999999999</v>
+        <v>121185.442</v>
       </c>
       <c r="O34">
-        <v>8.9952099323272708E-4</v>
+        <v>0.39921218156814581</v>
       </c>
       <c r="P34">
-        <v>3.5339999999999998</v>
+        <v>1366.9960000000001</v>
       </c>
       <c r="Q34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="R34" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S34" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -2883,58 +2859,58 @@
         <v>2022</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="F35">
-        <v>5.6758336424952711E-2</v>
+        <v>0.18842217678940471</v>
       </c>
       <c r="G35">
-        <v>4.3036028759487428E-2</v>
+        <v>11422.152356973709</v>
       </c>
       <c r="H35">
-        <v>0.1051164331018848</v>
+        <v>27898.85472057349</v>
       </c>
       <c r="I35">
-        <v>8.3724617164398871E-2</v>
+        <v>0.3236120898438461</v>
       </c>
       <c r="J35">
-        <v>0.67791694184165607</v>
+        <v>0.58224702569154585</v>
       </c>
       <c r="K35">
-        <v>0.68878093625396497</v>
+        <v>58808.860480769821</v>
       </c>
       <c r="L35">
-        <v>0.75823273672565683</v>
+        <v>60619.999999999993</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
       <c r="N35">
-        <v>2283611510.3860002</v>
+        <v>491.75299999999999</v>
       </c>
       <c r="O35">
-        <v>497999.61847682373</v>
+        <v>1.729859590530395E-3</v>
       </c>
       <c r="P35">
-        <v>3294090.702</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="Q35" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="R35" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -2942,58 +2918,58 @@
         <v>2022</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F36">
-        <v>9.730948941140756E-2</v>
+        <v>5.2998865280422289E-2</v>
       </c>
       <c r="G36">
-        <v>1.0833328246400891E-2</v>
+        <v>4.1918919807496818E-2</v>
       </c>
       <c r="H36">
-        <v>2.646063906704017E-2</v>
+        <v>0.1023878702719896</v>
       </c>
       <c r="I36">
-        <v>0.2348754375481461</v>
+        <v>8.3724617164398871E-2</v>
       </c>
       <c r="J36">
-        <v>0.41430253596211192</v>
+        <v>0.63301412506139598</v>
       </c>
       <c r="K36">
-        <v>0.20600941676666759</v>
+        <v>0.68878093625396497</v>
       </c>
       <c r="L36">
-        <v>0.11132858996515201</v>
+        <v>0.79093994910456344</v>
       </c>
       <c r="M36">
-        <v>0</v>
+        <v>595700</v>
       </c>
       <c r="N36">
-        <v>10839748.037</v>
+        <v>2283611510.3860002</v>
       </c>
       <c r="O36">
-        <v>1.5216030165553091E-3</v>
+        <v>3960121.8994090622</v>
       </c>
       <c r="P36">
-        <v>3692.3130000000001</v>
+        <v>41827423.749999993</v>
       </c>
       <c r="Q36" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="R36" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -3001,58 +2977,58 @@
         <v>2022</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F37">
-        <v>0.28200201008689302</v>
+        <v>0.14620933153267379</v>
       </c>
       <c r="G37">
-        <v>37.063993622830083</v>
+        <v>2.820565936115995E-2</v>
       </c>
       <c r="H37">
-        <v>90.529607829672457</v>
+        <v>6.8892934380668264E-2</v>
       </c>
       <c r="I37">
-        <v>0.56200449257414731</v>
+        <v>0.2348754375481461</v>
       </c>
       <c r="J37">
-        <v>0.50177892492503062</v>
+        <v>0.62249732479030695</v>
       </c>
       <c r="K37">
-        <v>102.0320898939423</v>
+        <v>0.20600941676666759</v>
       </c>
       <c r="L37">
-        <v>131.43166465873631</v>
+        <v>0.19291285354694859</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
       <c r="N37">
-        <v>341701.06699999998</v>
+        <v>10839748.037</v>
       </c>
       <c r="O37">
-        <v>150.25054102305171</v>
+        <v>0.30736380934417251</v>
       </c>
       <c r="P37">
-        <v>454.03300000000002</v>
+        <v>60333.252999999997</v>
       </c>
       <c r="Q37" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="R37" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S37" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -3060,55 +3036,58 @@
         <v>2022</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E38" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="F38">
-        <v>0.196076989403597</v>
+        <v>0.20661224878281609</v>
       </c>
       <c r="G38">
-        <v>4.8346402873259269</v>
+        <v>5.0786812152556937</v>
       </c>
       <c r="H38">
-        <v>11.80871369834138</v>
+        <v>12.40478895468566</v>
       </c>
       <c r="I38">
-        <v>0.52826176887391274</v>
+        <v>0.56200449257414731</v>
       </c>
       <c r="J38">
-        <v>0.37117391595755878</v>
+        <v>0.36763451451512552</v>
       </c>
       <c r="K38">
-        <v>23.70568292430087</v>
+        <v>102.0320898939423</v>
       </c>
       <c r="L38">
-        <v>24.656846792840629</v>
+        <v>24.580736356024239</v>
       </c>
       <c r="M38">
         <v>0</v>
       </c>
       <c r="N38">
-        <v>181161.66</v>
+        <v>341701.06699999998</v>
       </c>
       <c r="O38">
-        <v>1.415946006774902E-3</v>
+        <v>8.8975090697407722E-2</v>
       </c>
       <c r="P38">
-        <v>46.707999999999991</v>
+        <v>361.863</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>85</v>
       </c>
       <c r="R38" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -3116,58 +3095,55 @@
         <v>2022</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E39" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F39">
-        <v>0.44577637535621262</v>
+        <v>0.22820976442673871</v>
       </c>
       <c r="G39">
-        <v>251360.4313361705</v>
+        <v>27.59312512092006</v>
       </c>
       <c r="H39">
-        <v>613953.30207331525</v>
+        <v>67.39680622147803</v>
       </c>
       <c r="I39">
-        <v>0.69971340783873703</v>
+        <v>0.52826176887391274</v>
       </c>
       <c r="J39">
-        <v>0.63708422671664844</v>
+        <v>0.43200128775779068</v>
       </c>
       <c r="K39">
-        <v>405401.53851634171</v>
+        <v>23.70568292430087</v>
       </c>
       <c r="L39">
-        <v>563871.13636363635</v>
+        <v>120.911237914091</v>
       </c>
       <c r="M39">
         <v>0</v>
       </c>
       <c r="N39">
-        <v>56.145000000000003</v>
+        <v>181161.66</v>
       </c>
       <c r="O39">
-        <v>2.8318920135498049E-3</v>
+        <v>2.1239190101623542E-3</v>
       </c>
       <c r="P39">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>103</v>
+        <v>6.3089999999999993</v>
       </c>
       <c r="R39" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -3175,58 +3151,58 @@
         <v>2022</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="F40">
-        <v>7.4775183427112812E-2</v>
+        <v>0.32083889140613692</v>
       </c>
       <c r="G40">
-        <v>5.7587099455044388</v>
+        <v>8299.9187841673865</v>
       </c>
       <c r="H40">
-        <v>14.065773868745451</v>
+        <v>20272.731540887631</v>
       </c>
       <c r="I40">
-        <v>0.1970920899125283</v>
+        <v>0.69971340783873703</v>
       </c>
       <c r="J40">
-        <v>0.37939210782278932</v>
+        <v>0.45852900317737039</v>
       </c>
       <c r="K40">
-        <v>19.465639990710269</v>
+        <v>405401.53851634171</v>
       </c>
       <c r="L40">
-        <v>77.0136518771331</v>
+        <v>25869.428571428569</v>
       </c>
       <c r="M40">
         <v>0</v>
       </c>
       <c r="N40">
-        <v>6118.5810000000001</v>
+        <v>56.145000000000003</v>
       </c>
       <c r="O40">
-        <v>1.9960609078407288E-3</v>
+        <v>3.2785606384277342E-4</v>
       </c>
       <c r="P40">
-        <v>0.29299999999999998</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="Q40" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="R40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -3234,58 +3210,58 @@
         <v>2022</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="E41" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="F41">
-        <v>8.0973882870842631E-2</v>
+        <v>7.4218281287803209E-2</v>
       </c>
       <c r="G41">
-        <v>31.306527464939531</v>
+        <v>1.0037732183240751</v>
       </c>
       <c r="H41">
-        <v>76.466871939134492</v>
+        <v>2.451737843728564</v>
       </c>
       <c r="I41">
-        <v>0.11857763803203181</v>
+        <v>0.1970920899125283</v>
       </c>
       <c r="J41">
-        <v>0.68287650365382424</v>
+        <v>0.37656651426620991</v>
       </c>
       <c r="K41">
-        <v>2.80479408211766</v>
+        <v>19.465639990710269</v>
       </c>
       <c r="L41">
-        <v>386.625</v>
+        <v>13.52460877437526</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
       <c r="N41">
-        <v>1367768.7279999999</v>
+        <v>6118.5810000000001</v>
       </c>
       <c r="O41">
-        <v>5.0720100551843639E-4</v>
+        <v>0.44380087982863181</v>
       </c>
       <c r="P41">
-        <v>8.0000000000000002E-3</v>
+        <v>69.588999999999984</v>
       </c>
       <c r="Q41" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="R41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -3293,55 +3269,58 @@
         <v>2022</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E42" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="F42">
-        <v>0.18778177577413149</v>
+        <v>4.2989345582177839E-2</v>
       </c>
       <c r="G42">
-        <v>4.1561578068020806E-3</v>
+        <v>0.48345060280210961</v>
       </c>
       <c r="H42">
-        <v>1.015150553275145E-2</v>
+        <v>1.1808385767079099</v>
       </c>
       <c r="I42">
-        <v>0.32917101207844429</v>
+        <v>0.11857763803203181</v>
       </c>
       <c r="J42">
-        <v>0.57046874993166607</v>
+        <v>0.36254175994435778</v>
       </c>
       <c r="K42">
-        <v>0.2132337962898988</v>
+        <v>2.80479408211766</v>
       </c>
       <c r="L42">
-        <v>2.213291353576936E-2</v>
+        <v>11.24582373271889</v>
       </c>
       <c r="M42">
         <v>0</v>
       </c>
       <c r="N42">
-        <v>1309045246.648</v>
+        <v>1367768.7279999999</v>
       </c>
       <c r="O42">
-        <v>1369.809134340227</v>
+        <v>8.7745773954689493E-2</v>
       </c>
       <c r="P42">
-        <v>2529724.0649999999</v>
+        <v>69.44</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>107</v>
       </c>
       <c r="R42" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S42" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -3349,58 +3328,55 @@
         <v>2022</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F43">
-        <v>2.6131127154330469E-2</v>
+        <v>0.15958068029866571</v>
       </c>
       <c r="G43">
-        <v>7.3009217689318472E-3</v>
+        <v>5.3217886133280261E-2</v>
       </c>
       <c r="H43">
-        <v>1.783265967673266E-2</v>
+        <v>0.12998584044117789</v>
       </c>
       <c r="I43">
-        <v>8.4589307893588359E-2</v>
+        <v>0.32917101207844429</v>
       </c>
       <c r="J43">
-        <v>0.30891761388097538</v>
+        <v>0.48479566682085667</v>
       </c>
       <c r="K43">
-        <v>0.31135226168540892</v>
+        <v>0.2132337962898988</v>
       </c>
       <c r="L43">
-        <v>0.27939559307230011</v>
+        <v>0.3334857705436492</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
       <c r="N43">
-        <v>36083553.387999997</v>
+        <v>1309045246.648</v>
       </c>
       <c r="O43">
-        <v>0.13213923209905629</v>
+        <v>674240.75114424329</v>
       </c>
       <c r="P43">
-        <v>1202736.909</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>89</v>
+        <v>6881154.5279999999</v>
       </c>
       <c r="R43" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -3408,58 +3384,58 @@
         <v>2022</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="E44" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="F44">
-        <v>9.6257244351926105E-2</v>
+        <v>1.055419248550221E-2</v>
       </c>
       <c r="G44">
-        <v>60.93636770030669</v>
+        <v>3.5151596324283141E-3</v>
       </c>
       <c r="H44">
-        <v>148.83839897585921</v>
+        <v>8.5858535974497659E-3</v>
       </c>
       <c r="I44">
-        <v>0.18845843476299359</v>
+        <v>8.4589307893588359E-2</v>
       </c>
       <c r="J44">
-        <v>0.51076113665583478</v>
+        <v>0.12476981723008269</v>
       </c>
       <c r="K44">
-        <v>261.68332735871081</v>
+        <v>0.31135226168540892</v>
       </c>
       <c r="L44">
-        <v>633.05747126436779</v>
+        <v>0.33305813185205019</v>
       </c>
       <c r="M44">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="N44">
-        <v>3135.4839999999999</v>
+        <v>36083553.387999997</v>
       </c>
       <c r="O44">
-        <v>2.130244223177433E-2</v>
+        <v>1.751365072055161</v>
       </c>
       <c r="P44">
-        <v>0.17399999999999999</v>
+        <v>183241.50399999999</v>
       </c>
       <c r="Q44" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="R44" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -3467,58 +3443,58 @@
         <v>2022</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E45" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F45">
-        <v>0.25906196717346491</v>
+        <v>8.7407807280895394E-2</v>
       </c>
       <c r="G45">
-        <v>57.775307377133693</v>
+        <v>33.936770908428933</v>
       </c>
       <c r="H45">
-        <v>141.11744061678701</v>
+        <v>82.891298563495681</v>
       </c>
       <c r="I45">
-        <v>0.55633613003249516</v>
+        <v>0.18845843476299359</v>
       </c>
       <c r="J45">
-        <v>0.46565727657905898</v>
+        <v>0.46380416663663759</v>
       </c>
       <c r="K45">
-        <v>44.35008459639068</v>
+        <v>261.68332735871081</v>
       </c>
       <c r="L45">
-        <v>223.01732673267321</v>
+        <v>388.25789096126249</v>
       </c>
       <c r="M45">
         <v>0</v>
       </c>
       <c r="N45">
-        <v>6056.9960000000001</v>
+        <v>3135.4839999999999</v>
       </c>
       <c r="O45">
-        <v>0.1904447379112244</v>
+        <v>0.16179712076038119</v>
       </c>
       <c r="P45">
-        <v>0.80800000000000005</v>
+        <v>8.3640000000000008</v>
       </c>
       <c r="Q45" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="R45" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -3526,58 +3502,58 @@
         <v>2022</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F46">
-        <v>7.2123604919420048E-2</v>
+        <v>0.21773413249906021</v>
       </c>
       <c r="G46">
-        <v>5.784313114537488</v>
+        <v>20.025169873958951</v>
       </c>
       <c r="H46">
-        <v>14.128310164087649</v>
+        <v>48.911911486392327</v>
       </c>
       <c r="I46">
-        <v>0.1370736247595076</v>
+        <v>0.55633613003249516</v>
       </c>
       <c r="J46">
-        <v>0.52616690516471865</v>
+        <v>0.391371548143642</v>
       </c>
       <c r="K46">
-        <v>12.220581158394211</v>
+        <v>44.35008459639068</v>
       </c>
       <c r="L46">
-        <v>80.2</v>
+        <v>91.970742685671411</v>
       </c>
       <c r="M46">
         <v>0</v>
       </c>
       <c r="N46">
-        <v>101999.215</v>
+        <v>6056.9960000000001</v>
       </c>
       <c r="O46">
-        <v>8.6619035005569469E-4</v>
+        <v>0.1587539147272706</v>
       </c>
       <c r="P46">
-        <v>5.0000000000000001E-3</v>
+        <v>11.997</v>
       </c>
       <c r="Q46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="R46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -3585,58 +3561,58 @@
         <v>2022</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="F47">
-        <v>0.1016454191103808</v>
+        <v>4.8285130299124478E-2</v>
       </c>
       <c r="G47">
-        <v>0.36799623220549721</v>
+        <v>1.4556090762801139</v>
       </c>
       <c r="H47">
-        <v>0.89883877391561429</v>
+        <v>3.5553567208629522</v>
       </c>
       <c r="I47">
-        <v>0.17493243990142021</v>
+        <v>0.1370736247595076</v>
       </c>
       <c r="J47">
-        <v>0.58105528721637367</v>
+        <v>0.35225690123712422</v>
       </c>
       <c r="K47">
-        <v>0.5800488353131279</v>
+        <v>12.220581158394211</v>
       </c>
       <c r="L47">
-        <v>3.620391705069125</v>
+        <v>30.146114699549809</v>
       </c>
       <c r="M47">
         <v>0</v>
       </c>
       <c r="N47">
-        <v>6817189.8300000001</v>
+        <v>101999.215</v>
       </c>
       <c r="O47">
-        <v>0.73391985498517753</v>
+        <v>0.30432060331106181</v>
       </c>
       <c r="P47">
-        <v>3.472</v>
+        <v>51.09</v>
       </c>
       <c r="Q47" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="R47" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S47" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -3644,58 +3620,58 @@
         <v>2022</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E48" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F48">
-        <v>0.2332876633604975</v>
+        <v>9.5440078102655743E-2</v>
       </c>
       <c r="G48">
-        <v>12.06019966193236</v>
+        <v>4.8063619965479677E-2</v>
       </c>
       <c r="H48">
-        <v>29.457299093365169</v>
+        <v>0.1173964336015081</v>
       </c>
       <c r="I48">
-        <v>0.60070175127737535</v>
+        <v>0.17493243990142021</v>
       </c>
       <c r="J48">
-        <v>0.38835855374887429</v>
+        <v>0.54558250120125884</v>
       </c>
       <c r="K48">
-        <v>19.018153843262169</v>
+        <v>0.5800488353131279</v>
       </c>
       <c r="L48">
-        <v>51.696688492677957</v>
+        <v>0.50359996472113377</v>
       </c>
       <c r="M48">
         <v>0</v>
       </c>
       <c r="N48">
-        <v>32134.628000000001</v>
+        <v>6817189.8300000001</v>
       </c>
       <c r="O48">
-        <v>1.6230432176589961E-2</v>
+        <v>0.25030603784322741</v>
       </c>
       <c r="P48">
-        <v>90.411999999999992</v>
+        <v>50251.048000000003</v>
       </c>
       <c r="Q48" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="R48" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -3703,58 +3679,58 @@
         <v>2022</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E49" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="F49">
-        <v>0.21221088453673109</v>
+        <v>0.25322531224567008</v>
       </c>
       <c r="G49">
-        <v>7.0883328647411608</v>
+        <v>11.244881646025201</v>
       </c>
       <c r="H49">
-        <v>17.31340667013091</v>
+        <v>27.465867166529371</v>
       </c>
       <c r="I49">
-        <v>0.50212014067497002</v>
+        <v>0.60070175127737535</v>
       </c>
       <c r="J49">
-        <v>0.42262970023761381</v>
+        <v>0.4215491493194311</v>
       </c>
       <c r="K49">
-        <v>10.538124362093701</v>
+        <v>19.018153843262169</v>
       </c>
       <c r="L49">
-        <v>33.402305825242713</v>
+        <v>44.406625650108069</v>
       </c>
       <c r="M49">
         <v>0</v>
       </c>
       <c r="N49">
-        <v>163469.345</v>
+        <v>32134.628000000001</v>
       </c>
       <c r="O49">
-        <v>3.043206033110619E-3</v>
+        <v>0.1656730553507805</v>
       </c>
       <c r="P49">
-        <v>1.6479999999999999</v>
+        <v>151.321</v>
       </c>
       <c r="Q49" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="R49" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S49" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -3762,58 +3738,58 @@
         <v>2022</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="E50" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="F50">
-        <v>5.3175132342682632E-2</v>
+        <v>0.1551917635488646</v>
       </c>
       <c r="G50">
-        <v>5.5735997452560762E-2</v>
+        <v>13.65149104705991</v>
       </c>
       <c r="H50">
-        <v>0.13613638192156241</v>
+        <v>33.344062794662527</v>
       </c>
       <c r="I50">
-        <v>0.13888223945297021</v>
+        <v>0.24703176337277891</v>
       </c>
       <c r="J50">
-        <v>0.38287928357239209</v>
+        <v>0.62822594726280301</v>
       </c>
       <c r="K50">
-        <v>1.2386366822495449</v>
+        <v>92.139652638840474</v>
       </c>
       <c r="L50">
-        <v>1.048159073556693</v>
+        <v>87.96530650134352</v>
       </c>
       <c r="M50">
         <v>0</v>
       </c>
       <c r="N50">
-        <v>11885529.514</v>
+        <v>5346.1360000000004</v>
       </c>
       <c r="O50">
-        <v>158.08953705943529</v>
+        <v>3.5929096341133109E-3</v>
       </c>
       <c r="P50">
-        <v>35550.497000000003</v>
+        <v>3210.1979999999999</v>
       </c>
       <c r="Q50" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="R50" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S50" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
@@ -3821,91 +3797,177 @@
         <v>2022</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F51">
-        <v>6.6227370217873477E-2</v>
+        <v>0.2311520659285706</v>
       </c>
       <c r="G51">
-        <v>0.1860081913281782</v>
+        <v>4.9506790145769219</v>
       </c>
       <c r="H51">
-        <v>0.4543290392666775</v>
+        <v>12.092140804928629</v>
       </c>
       <c r="I51">
+        <v>0.50212014067497002</v>
+      </c>
+      <c r="J51">
+        <v>0.46035210939327542</v>
+      </c>
+      <c r="K51">
+        <v>10.538124362093701</v>
+      </c>
+      <c r="L51">
+        <v>21.41741193049408</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>163469.345</v>
+      </c>
+      <c r="O51">
+        <v>5.832811563462019E-2</v>
+      </c>
+      <c r="P51">
+        <v>456.99700000000001</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>104</v>
+      </c>
+      <c r="R51" t="s">
+        <v>120</v>
+      </c>
+      <c r="S51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2022</v>
+      </c>
+      <c r="B52" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" t="s">
+        <v>115</v>
+      </c>
+      <c r="F52">
+        <v>5.2948304018578807E-2</v>
+      </c>
+      <c r="G52">
+        <v>6.6754385142398245E-2</v>
+      </c>
+      <c r="H52">
+        <v>0.1630490326905788</v>
+      </c>
+      <c r="I52">
+        <v>0.13888223945297021</v>
+      </c>
+      <c r="J52">
+        <v>0.3812460414458449</v>
+      </c>
+      <c r="K52">
+        <v>1.2386366822495449</v>
+      </c>
+      <c r="L52">
+        <v>1.2607464276660321</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>11885529.514</v>
+      </c>
+      <c r="O52">
+        <v>1.4386118620634081E-3</v>
+      </c>
+      <c r="P52">
+        <v>214251.035</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>115</v>
+      </c>
+      <c r="R52" t="s">
+        <v>120</v>
+      </c>
+      <c r="S52" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2022</v>
+      </c>
+      <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" t="s">
+        <v>55</v>
+      </c>
+      <c r="E53" t="s">
+        <v>105</v>
+      </c>
+      <c r="F53">
+        <v>0.11135808900091571</v>
+      </c>
+      <c r="G53">
+        <v>0.28928756901876401</v>
+      </c>
+      <c r="H53">
+        <v>0.70659115797862837</v>
+      </c>
+      <c r="I53">
         <v>0.1947155986542316</v>
       </c>
-      <c r="J51">
-        <v>0.34012359911378992</v>
-      </c>
-      <c r="K51">
+      <c r="J53">
+        <v>0.57190122296601986</v>
+      </c>
+      <c r="K53">
         <v>1.778915108979497</v>
       </c>
-      <c r="L51">
-        <v>2.808630188942308</v>
-      </c>
-      <c r="M51">
-        <v>0</v>
-      </c>
-      <c r="N51">
+      <c r="L53">
+        <v>2.5978136982611559</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
         <v>1156475.79</v>
       </c>
-      <c r="O51">
-        <v>86.660871003885561</v>
-      </c>
-      <c r="P51">
-        <v>1692.6859999999999</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>106</v>
-      </c>
-      <c r="R51" t="s">
-        <v>123</v>
-      </c>
-      <c r="S51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>2022</v>
-      </c>
-      <c r="B52" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" s="9"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="2"/>
-      <c r="K52" s="7"/>
-    </row>
-    <row r="53" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>2022</v>
-      </c>
-      <c r="B53" t="s">
-        <v>18</v>
-      </c>
-      <c r="C53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" s="10"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="2"/>
-      <c r="K53" s="8"/>
+      <c r="O53">
+        <v>449.24872582890538</v>
+      </c>
+      <c r="P53">
+        <v>17983.611000000001</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>105</v>
+      </c>
+      <c r="R53" t="s">
+        <v>120</v>
+      </c>
+      <c r="S53" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>